<commit_message>
research log and other things
</commit_message>
<xml_diff>
--- a/hours_christophe.xlsx
+++ b/hours_christophe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7CFAB9-FC44-404F-931D-6E09B4700744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B8094-6FF7-FD4B-96B2-B8E848FFCCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-13700" windowWidth="38400" windowHeight="19640" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
+    <workbookView xWindow="29400" yWindow="-13700" windowWidth="38400" windowHeight="19620" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,6 +560,10 @@
         <f>E2-C2-D2</f>
         <v>7.75</v>
       </c>
+      <c r="H2">
+        <f>SUM(F2:F123)</f>
+        <v>174.75</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1097,9 +1101,12 @@
       <c r="D30">
         <v>1</v>
       </c>
+      <c r="E30">
+        <v>18</v>
+      </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1109,9 +1116,18 @@
       <c r="B31" s="2">
         <v>45443</v>
       </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>18</v>
+      </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1121,6 +1137,15 @@
       <c r="B32" s="2">
         <v>45444</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
       <c r="F32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1133,6 +1158,15 @@
       <c r="B33" s="2">
         <v>45445</v>
       </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
       <c r="F33">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1145,9 +1179,18 @@
       <c r="B34" s="2">
         <v>45446</v>
       </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>0.25</v>
+      </c>
+      <c r="E34">
+        <v>17</v>
+      </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1157,9 +1200,18 @@
       <c r="B35" s="2">
         <v>45447</v>
       </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>18</v>
+      </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1169,9 +1221,15 @@
       <c r="B36" s="2">
         <v>45448</v>
       </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
upload temp sensor hobos
</commit_message>
<xml_diff>
--- a/hours_christophe.xlsx
+++ b/hours_christophe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B8094-6FF7-FD4B-96B2-B8E848FFCCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F62AA5-3840-BC4B-B57C-C6CB659E0A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-13700" windowWidth="38400" windowHeight="19620" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="14">
   <si>
     <t>Day of week</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Wednesday</t>
+  </si>
+  <si>
+    <t>week total</t>
   </si>
 </sst>
 </file>
@@ -509,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4659F124-5BD7-4242-BAAC-21A20EBB7F00}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,6 +540,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
@@ -560,9 +566,13 @@
         <f>E2-C2-D2</f>
         <v>7.75</v>
       </c>
+      <c r="G2">
+        <f>SUM(F2:F4)</f>
+        <v>21.25</v>
+      </c>
       <c r="H2">
         <f>SUM(F2:F123)</f>
-        <v>174.75</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -640,6 +650,10 @@
         <f t="shared" si="0"/>
         <v>7.25</v>
       </c>
+      <c r="G6">
+        <f>SUM(F6:F12)</f>
+        <v>44.5</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -769,6 +783,10 @@
         <f t="shared" si="0"/>
         <v>8.75</v>
       </c>
+      <c r="G13">
+        <f>SUM(F13:F19)</f>
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -833,7 +851,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -854,7 +872,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -866,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -878,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -898,8 +916,12 @@
         <f t="shared" si="0"/>
         <v>9.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f>SUM(F20:F26)</f>
+        <v>45.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -920,7 +942,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -941,7 +963,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -962,7 +984,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -983,7 +1005,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1045,8 +1067,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f>SUM(F27:F33)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1088,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1130,7 +1156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1151,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1172,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1192,8 +1218,12 @@
         <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <f>SUM(F34:F40)</f>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1214,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1227,36 +1257,57 @@
       <c r="D36">
         <v>0</v>
       </c>
+      <c r="E36">
+        <v>19</v>
+      </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="2">
         <v>45449</v>
       </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>19</v>
+      </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="2">
         <v>45450</v>
       </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>0.25</v>
+      </c>
+      <c r="E38">
+        <v>18</v>
+      </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1291,8 +1342,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <f>SUM(F41:F47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1316,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1352,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1375,8 +1430,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <f>SUM(F48:F54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1424,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -1436,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1448,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1459,8 +1518,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <f>SUM(F55:F61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1472,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -1484,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1496,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1508,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -1520,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1543,8 +1606,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <f>SUM(F62:F68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
dailylog updated, data and tree inventory
</commit_message>
<xml_diff>
--- a/hours_christophe.xlsx
+++ b/hours_christophe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F62AA5-3840-BC4B-B57C-C6CB659E0A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D572FC38-9152-8843-A7DE-07CFE7126712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-13700" windowWidth="38400" windowHeight="19620" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4659F124-5BD7-4242-BAAC-21A20EBB7F00}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,7 @@
       </c>
       <c r="H2">
         <f>SUM(F2:F123)</f>
-        <v>212.5</v>
+        <v>227.25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="G34">
         <f>SUM(F34:F40)</f>
-        <v>39.5</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,9 +1326,18 @@
       <c r="B40" s="2">
         <v>45452</v>
       </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>18</v>
+      </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1338,13 +1347,22 @@
       <c r="B41" s="2">
         <v>45453</v>
       </c>
+      <c r="C41">
+        <v>10.5</v>
+      </c>
+      <c r="D41">
+        <v>0.25</v>
+      </c>
+      <c r="E41">
+        <v>19.5</v>
+      </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.75</v>
       </c>
       <c r="G41">
         <f>SUM(F41:F47)</f>
-        <v>0</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
hours from last week
</commit_message>
<xml_diff>
--- a/hours_christophe.xlsx
+++ b/hours_christophe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D572FC38-9152-8843-A7DE-07CFE7126712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6871A2B-B911-3C49-A8C0-6BAF705803C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
+    <workbookView xWindow="-32920" yWindow="-3240" windowWidth="29400" windowHeight="17220" xr2:uid="{D685910A-BF7B-574C-817F-C963C9310E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,7 @@
       </c>
       <c r="H2">
         <f>SUM(F2:F123)</f>
-        <v>227.25</v>
+        <v>238.75</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1372,6 +1372,15 @@
       <c r="B42" s="2">
         <v>45454</v>
       </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
       <c r="F42">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1384,6 +1393,15 @@
       <c r="B43" s="2">
         <v>45455</v>
       </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
       <c r="F43">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1396,6 +1414,15 @@
       <c r="B44" s="2">
         <v>45456</v>
       </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
       <c r="F44">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1408,6 +1435,15 @@
       <c r="B45" s="2">
         <v>45457</v>
       </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
       <c r="F45">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1420,6 +1456,15 @@
       <c r="B46" s="2">
         <v>45458</v>
       </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
       <c r="F46">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1432,6 +1477,15 @@
       <c r="B47" s="2">
         <v>45459</v>
       </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
       <c r="F47">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1444,13 +1498,22 @@
       <c r="B48" s="2">
         <v>45460</v>
       </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
       <c r="F48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G48">
         <f>SUM(F48:F54)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1460,6 +1523,15 @@
       <c r="B49" s="2">
         <v>45461</v>
       </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
       <c r="F49">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1472,9 +1544,18 @@
       <c r="B50" s="2">
         <v>45462</v>
       </c>
+      <c r="C50">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>16</v>
+      </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1484,9 +1565,18 @@
       <c r="B51" s="2">
         <v>45463</v>
       </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0.25</v>
+      </c>
+      <c r="E51">
+        <v>17.5</v>
+      </c>
       <c r="F51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1496,9 +1586,18 @@
       <c r="B52" s="2">
         <v>45464</v>
       </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>0.25</v>
+      </c>
+      <c r="E52">
+        <v>18</v>
+      </c>
       <c r="F52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1532,13 +1631,16 @@
       <c r="B55" s="2">
         <v>45467</v>
       </c>
+      <c r="C55">
+        <v>8.5</v>
+      </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8.5</v>
       </c>
       <c r="G55">
         <f>SUM(F55:F61)</f>
-        <v>0</v>
+        <v>-8.5</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>